<commit_message>
Classifying each test case in a separate class and updating Scenario of day 9
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -23,13 +23,13 @@
     <t>Order Id</t>
   </si>
   <si>
-    <t>leatha.beer@gmail.com</t>
+    <t>armand.mcclure@yahoo.com</t>
   </si>
   <si>
-    <t>2bbdhwmy</t>
+    <t>bpvi0qvuw1uqie</t>
   </si>
   <si>
-    <t>100023193</t>
+    <t>100023200</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
initializing the page classes in a @BeforeMethod to make code readable and act as dependency injection container
</commit_message>
<xml_diff>
--- a/UserData.xlsx
+++ b/UserData.xlsx
@@ -23,13 +23,13 @@
     <t>Order Id</t>
   </si>
   <si>
-    <t>armand.mcclure@yahoo.com</t>
+    <t>donald.schumm@yahoo.com</t>
   </si>
   <si>
-    <t>bpvi0qvuw1uqie</t>
+    <t>g4ziplkh</t>
   </si>
   <si>
-    <t>100023200</t>
+    <t>100023203</t>
   </si>
 </sst>
 </file>

</xml_diff>